<commit_message>
Ajout des espèces alouette lulu, bergeronnette grise, sylvine, lucilie soyeuse et cicadelle du rhododendron
</commit_message>
<xml_diff>
--- a/inst/extdata/Especes.xlsx
+++ b/inst/extdata/Especes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Especes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiba\Documents\Especes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="10910" windowHeight="5960"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="10800" windowHeight="5970"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="277">
   <si>
     <t>Nom vernaculaire</t>
   </si>
@@ -1053,6 +1053,155 @@
   <si>
     <t xml:space="preserve">Net dimorphisme sexuel. Mâle avec plumage plutôt sobre. Tête remarquable, avec calotte grise, nuque châtaine, joues blanc sale et gorge noire se prolongeant en bavette sur la poitrine. L'œil sombre est inclus dans une zone lorale noire qui se poursuit par dessous. Dessus présente des teintes chaudes, marron et chamois, avec stries noirâtres longitudinales. Extrémité blanche des couvertures moyennes forme une petite barre alaire. Gris clair du dos et croupion ne se voit que lorsque les ailes les découvrent. Rectrices brun-gris bordées de beige. Parties inférieures blanchâtres, teintées de crème ou de gris. Bec fort et conique noir. Pattes roses. &lt;br&gt;
 Femelle avec plumage plus discret, dépourvu des teintes chaudes. Parties supérieures, tête comprise, apparaissent brunes, chamois clair ou beige. Manteau strié en long de noirâtre. Barre alaire blanche plus fine. Dos et croupion bruns.Tête brune se caractérise par un sourcil pâle qui va de l'œil aux côtés de la nuque. Bec brunâtre, avec souvent du jaune à la base de la mandibule inférieure. Parties inférieures identiques au mâle mais paraissent souvent striées. </t>
+  </si>
+  <si>
+    <t>Hepialidae</t>
+  </si>
+  <si>
+    <t>Triodia</t>
+  </si>
+  <si>
+    <t>Triodia sylvina</t>
+  </si>
+  <si>
+    <t>La sylvine</t>
+  </si>
+  <si>
+    <t>Envergure entre 32 et 48 mm</t>
+  </si>
+  <si>
+    <t>Partout en France sauf en Corse. Affectionne les prairies, les espaces cultivés, les jardins. L’activité est crépusculaire et nocturne dans les deux sexes mais les femelles, beaucoup plus grosses que les mâles, volent peu, après avoir pondu. Les chenilles, endophytes, se développent en deux ans dans les racines de nombreuses plantes basses.</t>
+  </si>
+  <si>
+    <t>hepialus_sylvina_1.jpg</t>
+  </si>
+  <si>
+    <t>hepialus_sylvina_2.jpg</t>
+  </si>
+  <si>
+    <t>hepialus_sylvina_3.jpg</t>
+  </si>
+  <si>
+    <t>La lucilie soyeuse</t>
+  </si>
+  <si>
+    <t>Lucilia sericata</t>
+  </si>
+  <si>
+    <t>Lucilia</t>
+  </si>
+  <si>
+    <t>Entre 10 et 14 mm</t>
+  </si>
+  <si>
+    <t>Grosse mouche verte aux reflets métalliques, parfois dorés ou cuivrés. Les antennes ont une arista plumeuse. L’espace entre les yeux mesure plus de deux fois la taille du 3ème article antennaire. Les palpes sont orangés. Les gènes (joues) sont noirs, partiellement rougeâtres, et recouverts d’une pruinosité argentée. Les ailes sont hyalines, avec des nervures brun clair. La nervure médiane est anguleuse et très fortement courbée vers la nervure radiale. La basicosta est jaune. Les pattes antérieures sont noires. Le thorax porte 3 soies acrosticales post-suturales et 2 soies acrosticales pré-suturales.</t>
+  </si>
+  <si>
+    <t>Calliphoridae</t>
+  </si>
+  <si>
+    <t>lucilia_sericata_1.jpg</t>
+  </si>
+  <si>
+    <t>lucilia_sericata_2.jpg</t>
+  </si>
+  <si>
+    <t>lucilia_sericata_3.jpg</t>
+  </si>
+  <si>
+    <t>Motacillidae</t>
+  </si>
+  <si>
+    <t>Motacilla</t>
+  </si>
+  <si>
+    <t>Motacilla alba</t>
+  </si>
+  <si>
+    <t>Bergeronnette grise</t>
+  </si>
+  <si>
+    <t>Entre 17 et 18 cm.</t>
+  </si>
+  <si>
+    <t>Oiseau gris, noir et blanc. Le bec, l’oeil et le dessus de la calotte sont systématiquement noirs tout comme le dessus de la longue queue. Les épaules et le dessus du dos sont gris. Le ventre et le dessous sont blanc-gris. Pendant la période de nidification, la gorge et le jabot (partie sous la gorge) sont noirs alors que l’hiver la gorge devient blanche (mais le jabot reste noir comme un collier). Attention tout de même, dans le Nord-Ouest de la France, la sous-espèce dite de Yarrell est dominante.</t>
+  </si>
+  <si>
+    <t>Motacilla_alba_2.jpg</t>
+  </si>
+  <si>
+    <t>Motacilla_alba_3.jpg</t>
+  </si>
+  <si>
+    <t>Motacilla_alba_1.jpg</t>
+  </si>
+  <si>
+    <t>Hémiptères</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Auchenorrhyncha</t>
+  </si>
+  <si>
+    <t>Cicadellidae</t>
+  </si>
+  <si>
+    <t>La cicadelle du rhododendron</t>
+  </si>
+  <si>
+    <t>Graphocephala</t>
+  </si>
+  <si>
+    <t>Graphocephala fennahi</t>
+  </si>
+  <si>
+    <t>Entre 8 et 9,5 mm</t>
+  </si>
+  <si>
+    <t>La cicadelle du rhododenron présente des teintes vives, orange vif et vert. Il a un corps très allongé, avec des élytres longues, bordées en leur extrémité d’un brun très sombre et marquées d’une sorte de V orange vif (qui semble émettre des signaux lorsque l’insecte vole). La tête, jaune pâle, est triangulaire et plate, faisant un peu penser à celle d’un reptile avec les yeux sur le côté. Ses pattes sont très fines, jaune pâle comme la tête, avec des épines très visibles sur les tibias postérieurs.</t>
+  </si>
+  <si>
+    <t>Graphocephala_fennahi_1.jpg</t>
+  </si>
+  <si>
+    <t>Graphocephala_fennahi_2.jpg</t>
+  </si>
+  <si>
+    <t>Graphocephala_fennahi_3.jpg</t>
+  </si>
+  <si>
+    <t>Alaudidae</t>
+  </si>
+  <si>
+    <t>Lullula</t>
+  </si>
+  <si>
+    <t>Lullula arborea</t>
+  </si>
+  <si>
+    <t>Alouette lulu</t>
+  </si>
+  <si>
+    <t>15 cm</t>
+  </si>
+  <si>
+    <t>Lullula_arborea_1.jpg</t>
+  </si>
+  <si>
+    <t>16 cm</t>
+  </si>
+  <si>
+    <t>Lullula_arborea_2.jpg</t>
+  </si>
+  <si>
+    <t>Lullula_arborea_3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus petite que l'Alouette des champs. En comparaison, ses ailes sont plus larges et plus arrondie. Sa queue est nettement plus courte et le blanc est à l'extrémité et non sur les bords externes. Concernant le plumage, de nets sourcils blancs sur  la tête qui se rejoignent sur la nuque et des couvertures auriculaires roux chamois avec souvent une tache claire sous l'oeil. Le bord de l'aile au niveau de la main où se trouve un insigne caractéristique de l'espèce. L'alula est largement blanchâtre et juste en arrière, les couvertures primaires sont noires à la base et blanches à l'extrémité. Le bec plus fin, rose à la base de la mandibule inférieure, un ongle postérieur plus long.
+Autrement, le plumage est assez similaire. Parties supérieures brunes striées de brun noirâtre. Parties inférieures blanc crème avec des stries brun noirâtre, fines sur la poitrine et indistinctes sur les flancs. En revanche, en vue de dessous en vol, l'aspect est très différent de celui de l'Alouette des champs. Les rémiges noirâtres contrastent avec les couvertures blanches et la queue noire à bout blanc contraste avec les sous-caudales blanches. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus petite que l'Alouette des champs. Ses ailes sont plus larges et plus arrondie. Sa queue est nettement plus courte et le blanc est à l'extrémité et non sur les bords externes. Sur son plumage, de nets sourcils blancs sur  la tête se rejoignent sur la nuque et les couvertures auriculaires roux chamois avec tache claire sous l'oeil. Sur le bord de l'aile se trouve un insigne caractéristique de l'espèce. L'alula est blanchâtre et juste en arrière, les couvertures primaires sont noires à la base et blanches à l'extrémité. Le bec plus fin, rose à la base de la mandibule inférieure, un ongle postérieur plus long.
+Le plumage est assez similaire. Parties supérieures brunes striées de brun noirâtre. Parties inférieures blanc crème avec des stries brun noirâtre, fines sur la poitrine et indistinctes sur les flancs. En revanche, en vue de dessous en vol, l'aspect est très différent de celui de l'Alouette des champs. Les rémiges noirâtres contrastent avec les couvertures blanches, et la queue noire à bout blanc avec les sous-caudales blanches. </t>
   </si>
 </sst>
 </file>
@@ -1480,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K76"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:I22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,7 +1642,7 @@
     <col min="3" max="3" width="15.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.81640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="143.1796875" style="1" customWidth="1"/>
@@ -1627,7 +1776,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1635,31 +1784,29 @@
         <v>153</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>219</v>
+        <v>270</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1667,31 +1814,29 @@
         <v>153</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>219</v>
+        <v>272</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1699,28 +1844,26 @@
         <v>153</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="5" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
@@ -1746,16 +1889,16 @@
         <v>219</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1763,29 +1906,31 @@
         <v>153</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>154</v>
+        <v>215</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>157</v>
+        <v>218</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="J9" s="4"/>
+        <v>226</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="K9" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1793,29 +1938,31 @@
         <v>153</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>154</v>
+        <v>215</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>157</v>
+        <v>218</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="J10" s="4"/>
+        <v>226</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K10" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1823,29 +1970,31 @@
         <v>153</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>154</v>
+        <v>215</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>156</v>
+        <v>216</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>157</v>
+        <v>218</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>155</v>
+        <v>217</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="J11" s="4"/>
+        <v>225</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="K11" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1853,26 +2002,26 @@
         <v>153</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="5" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1883,26 +2032,26 @@
         <v>153</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="5" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1913,29 +2062,29 @@
         <v>153</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1943,28 +2092,26 @@
         <v>153</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>158</v>
+        <v>250</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="J15" s="4"/>
       <c r="K15" s="5" t="s">
-        <v>168</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -1975,28 +2122,26 @@
         <v>153</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>158</v>
+        <v>250</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="J16" s="4"/>
       <c r="K16" s="5" t="s">
-        <v>169</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2007,28 +2152,26 @@
         <v>153</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>165</v>
+        <v>246</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>164</v>
+        <v>247</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>166</v>
+        <v>249</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>163</v>
+        <v>248</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>158</v>
+        <v>250</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="J17" s="4"/>
       <c r="K17" s="5" t="s">
-        <v>170</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="87" x14ac:dyDescent="0.35">
@@ -2039,31 +2182,29 @@
         <v>153</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>158</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="J18" s="4"/>
       <c r="K18" s="5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2071,28 +2212,26 @@
         <v>153</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="J19" s="4"/>
       <c r="K19" s="5" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2103,31 +2242,29 @@
         <v>153</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>201</v>
+        <v>155</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>203</v>
+        <v>158</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="J20" s="4"/>
       <c r="K20" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
@@ -2135,31 +2272,29 @@
         <v>153</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="J21" s="4"/>
       <c r="K21" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -2167,28 +2302,26 @@
         <v>153</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="J22" s="4"/>
       <c r="K22" s="5" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2199,29 +2332,29 @@
         <v>153</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>158</v>
+        <v>210</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -2229,26 +2362,28 @@
         <v>153</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>158</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J24" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="K24" s="5" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2259,200 +2394,220 @@
         <v>153</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>158</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J25" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="K25" s="5" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>92</v>
+        <v>164</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>92</v>
+        <v>164</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>88</v>
+        <v>199</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>92</v>
+        <v>200</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>95</v>
+        <v>203</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>81</v>
+        <v>201</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>84</v>
+        <v>203</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>81</v>
+        <v>201</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>81</v>
+        <v>201</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I31" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>86</v>
+        <v>203</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2460,32 +2615,28 @@
         <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="J32" s="4"/>
+        <v>96</v>
+      </c>
       <c r="K32" s="1" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2493,32 +2644,28 @@
         <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33" s="4"/>
+        <v>96</v>
+      </c>
       <c r="K33" s="1" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2526,140 +2673,118 @@
         <v>122</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="J34" s="4"/>
+        <v>96</v>
+      </c>
       <c r="K34" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>106</v>
+        <v>82</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>106</v>
+        <v>82</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>106</v>
+        <v>82</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>122</v>
       </c>
@@ -2670,496 +2795,523 @@
         <v>101</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>102</v>
+        <v>242</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>104</v>
+        <v>239</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>106</v>
+        <v>237</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>103</v>
+        <v>238</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>105</v>
+        <v>240</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="J38" s="4"/>
       <c r="K38" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39" s="6"/>
+        <v>239</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="G39" s="3" t="s">
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>130</v>
+        <v>241</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>126</v>
+        <v>242</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F40" s="6"/>
+        <v>239</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="G40" s="3" t="s">
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>130</v>
+        <v>241</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F41" s="6"/>
+        <v>136</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>137</v>
+      </c>
       <c r="G41" s="3" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J52" s="4"/>
+      <c r="K52" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="100.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J53" s="4"/>
+      <c r="K53" s="1" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="100.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J42" s="4"/>
-      <c r="K42" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J43" s="4"/>
-      <c r="K43" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I44" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="4"/>
-      <c r="K44" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K46" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I47" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K47" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I48" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K48" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I49" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K49" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I50" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K50" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I51" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K51" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I52" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K52" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I53" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="K53" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3170,25 +3322,26 @@
         <v>119</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>185</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J54" s="4"/>
       <c r="K54" s="5" t="s">
-        <v>186</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3199,25 +3352,26 @@
         <v>119</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>185</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J55" s="4"/>
       <c r="K55" s="5" t="s">
-        <v>187</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3228,28 +3382,29 @@
         <v>119</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>183</v>
+        <v>11</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>185</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J56" s="4"/>
       <c r="K56" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>122</v>
       </c>
@@ -3257,28 +3412,28 @@
         <v>119</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>143</v>
+        <v>228</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>146</v>
+        <v>231</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>148</v>
+        <v>233</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>122</v>
       </c>
@@ -3286,28 +3441,28 @@
         <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>143</v>
+        <v>228</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>146</v>
+        <v>231</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="I58" s="10" t="s">
-        <v>148</v>
+        <v>233</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>122</v>
       </c>
@@ -3315,25 +3470,25 @@
         <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>143</v>
+        <v>228</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>146</v>
+        <v>231</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>144</v>
+        <v>230</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>147</v>
+        <v>232</v>
       </c>
       <c r="I59" s="10" t="s">
-        <v>148</v>
+        <v>233</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>152</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3344,26 +3499,28 @@
         <v>119</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="I60" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="J60" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="K60" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3374,29 +3531,31 @@
         <v>119</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="J61" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="K61" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -3404,125 +3563,127 @@
         <v>119</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="I62" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="J62" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="K62" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="8" t="s">
-        <v>50</v>
+      <c r="D63" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I63" s="10" t="s">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="8" t="s">
-        <v>50</v>
+      <c r="D64" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H64" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I64" s="10" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>31</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D65" s="8" t="s">
-        <v>50</v>
+      <c r="D65" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K65" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>122</v>
       </c>
@@ -3530,31 +3691,31 @@
         <v>119</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="J66" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K66" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="K66" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>122</v>
       </c>
@@ -3562,29 +3723,31 @@
         <v>119</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="H67" s="8" t="s">
-        <v>192</v>
+        <v>40</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I67" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="J67" s="4"/>
-      <c r="K67" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
@@ -3592,26 +3755,25 @@
         <v>119</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G68" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>192</v>
+        <v>40</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I68" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="J68" s="4"/>
-      <c r="K68" s="1" t="s">
-        <v>197</v>
+        <v>149</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
@@ -3622,264 +3784,716 @@
         <v>119</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>50</v>
+        <v>180</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>192</v>
+        <v>183</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="I69" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="J69" s="4"/>
-      <c r="K69" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>19</v>
+        <v>182</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="I70" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>19</v>
+        <v>182</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>31</v>
+        <v>185</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="I72" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>16</v>
+        <v>146</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>45</v>
+        <v>144</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="I73" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="J74" s="4"/>
+        <v>148</v>
+      </c>
       <c r="K74" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>114</v>
+        <v>13</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>194</v>
+        <v>99</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>114</v>
+        <v>13</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>115</v>
+        <v>15</v>
       </c>
       <c r="I76" s="10" t="s">
-        <v>194</v>
+        <v>99</v>
       </c>
       <c r="J76" s="4"/>
       <c r="K76" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="J77" s="4"/>
+      <c r="K77" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H78" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I78" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H79" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K79" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H80" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H81" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I81" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H82" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J82" s="4"/>
+      <c r="K82" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I83" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J83" s="4"/>
+      <c r="K83" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="J84" s="4"/>
+      <c r="K84" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K85" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K86" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K87" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="105.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I88" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K88" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I89" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J89" s="4"/>
+      <c r="K89" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J90" s="4"/>
+      <c r="K90" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J91" s="4"/>
+      <c r="K91" s="5" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3891,28 +4505,31 @@
   </autoFilter>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K52" r:id="rId1" display="https://www.trigobert.net/wp-content/uploads/2021/07/Polyommatus-icarus-4.jpg"/>
-    <hyperlink ref="K60" r:id="rId2" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
-    <hyperlink ref="K62" r:id="rId3" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
-    <hyperlink ref="K61" r:id="rId4" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
-    <hyperlink ref="B26" r:id="rId5" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
-    <hyperlink ref="B27" r:id="rId6" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
-    <hyperlink ref="B28" r:id="rId7" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
-    <hyperlink ref="C35" r:id="rId8" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="D35" r:id="rId9" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
-    <hyperlink ref="C36" r:id="rId10" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="C37" r:id="rId11" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="C38" r:id="rId12" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="D36" r:id="rId13" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
-    <hyperlink ref="D37" r:id="rId14" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
-    <hyperlink ref="D38" r:id="rId15" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
-    <hyperlink ref="C34" r:id="rId16" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="C33" r:id="rId17" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="C32" r:id="rId18" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
-    <hyperlink ref="D32" r:id="rId19" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
-    <hyperlink ref="D33:D34" r:id="rId20" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="K67" r:id="rId1" display="https://www.trigobert.net/wp-content/uploads/2021/07/Polyommatus-icarus-4.jpg"/>
+    <hyperlink ref="K75" r:id="rId2" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
+    <hyperlink ref="K77" r:id="rId3" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
+    <hyperlink ref="K76" r:id="rId4" display="https://quelestcetanimal-lagalerie.com/wp-content/uploads/2012/09/iphiclides-podalirius-1024x681.jpg"/>
+    <hyperlink ref="B32" r:id="rId5" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
+    <hyperlink ref="B33" r:id="rId6" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
+    <hyperlink ref="B34" r:id="rId7" display="https://quelestcetanimal-lagalerie.com/coleopteres/"/>
+    <hyperlink ref="C44" r:id="rId8" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="D44" r:id="rId9" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="C45" r:id="rId10" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C46" r:id="rId11" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C47" r:id="rId12" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="D45" r:id="rId13" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="D46" r:id="rId14" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="D47" r:id="rId15" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="C43" r:id="rId16" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C42" r:id="rId17" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C41" r:id="rId18" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="D41" r:id="rId19" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="D42:D43" r:id="rId20" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/syrphidae/"/>
+    <hyperlink ref="C40" r:id="rId21" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C39" r:id="rId22" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
+    <hyperlink ref="C38" r:id="rId23" tooltip="Brachycères" display="https://quelestcetanimal-lagalerie.com/dipteres/brachyceres/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>